<commit_message>
Tudo que foi feito ate antes da formatacao do sistema
</commit_message>
<xml_diff>
--- a/Secao03/FórmulaSomaeSubtotal.xlsx
+++ b/Secao03/FórmulaSomaeSubtotal.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Curso de Excel\Fórmulas Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\gabrielrstan\Aulas\Curso_de_Excel_do_Basico_ao_Avancado_Macro_e_VBA_plus_Power_BI\Secao03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA1F664-C715-4661-A078-457CE7B338F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="894" xr2:uid="{193F081A-02DB-4BD2-87B0-9E4D48AC40BC}"/>
+    <workbookView xWindow="-105" yWindow="375" windowWidth="23250" windowHeight="12570" tabRatio="894" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Professor" sheetId="17" r:id="rId1"/>
     <sheet name="Aluno" sheetId="20" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Aluno!$C$5:$D$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Aluno!$E$10:$F$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Professor!$E$10:$F$15</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -79,8 +78,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,12 +201,6 @@
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -231,6 +224,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,213 +544,213 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB5B962-C132-4CAD-B5CA-108538948F92}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="B1:N17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" style="13" customWidth="1"/>
-    <col min="7" max="8" width="5.21875" customWidth="1"/>
-    <col min="9" max="10" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.375" customWidth="1"/>
+    <col min="6" max="6" width="23.375" style="11" customWidth="1"/>
+    <col min="7" max="8" width="5.25" customWidth="1"/>
+    <col min="9" max="10" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="2:14" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="2:14" s="1" customFormat="1">
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="2:14" s="1" customFormat="1" ht="15.6" customHeight="1">
+      <c r="B2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="2:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="2:14" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B5" s="3" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="14.45" customHeight="1">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+    </row>
+    <row r="4" spans="2:14" s="1" customFormat="1" ht="14.45" customHeight="1">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+    </row>
+    <row r="5" spans="2:14" s="1" customFormat="1" ht="22.5">
+      <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="2:14" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B6" s="3" t="s">
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="2:14" s="1" customFormat="1" ht="22.5">
+      <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="9"/>
-    </row>
-    <row r="10" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E10" s="8" t="s">
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="2:14" s="1" customFormat="1">
+      <c r="F7" s="7"/>
+    </row>
+    <row r="10" spans="2:14" ht="27">
+      <c r="E10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="8" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E11" s="7" t="s">
+    <row r="11" spans="2:14" ht="27">
+      <c r="E11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="11">
-        <v>100</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="7" t="s">
+      <c r="F11" s="9">
+        <v>100</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E12" s="7" t="s">
+      <c r="J11" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="27">
+      <c r="E12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="11">
-        <v>100</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="7" t="s">
+      <c r="F12" s="9">
+        <v>100</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E13" s="7" t="s">
+      <c r="J12" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="27">
+      <c r="E13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="11">
-        <v>100</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="7" t="s">
+      <c r="F13" s="9">
+        <v>100</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E14" s="7" t="s">
+      <c r="J13" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="27">
+      <c r="E14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="11">
-        <v>100</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="7" t="s">
+      <c r="F14" s="9">
+        <v>100</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J14" s="11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E15" s="7" t="s">
+      <c r="J14" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="27">
+      <c r="E15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="11">
-        <v>100</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="7" t="s">
+      <c r="F15" s="9">
+        <v>100</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E16" s="6"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="5:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E17" s="14" t="s">
+      <c r="J15" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="27">
+      <c r="E16" s="4"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="5:10" ht="27">
+      <c r="E17" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="13">
         <f>SUM(F11:F15)</f>
         <v>500</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="14" t="s">
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="13">
         <f>SUBTOTAL(9,J11:J15)</f>
         <v>500</v>
       </c>
@@ -768,211 +767,218 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C4EF10-9EEC-4AA7-90F5-34C3B4B9BE36}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" style="13" customWidth="1"/>
-    <col min="7" max="8" width="5.21875" customWidth="1"/>
-    <col min="9" max="10" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.375" customWidth="1"/>
+    <col min="6" max="6" width="23.375" style="11" customWidth="1"/>
+    <col min="7" max="8" width="5.25" customWidth="1"/>
+    <col min="9" max="10" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="2:14" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="2:14" s="1" customFormat="1">
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="2:14" s="1" customFormat="1" ht="15.6" customHeight="1">
+      <c r="B2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="2:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="2:14" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B5" s="3" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="14.45" customHeight="1">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+    </row>
+    <row r="4" spans="2:14" s="1" customFormat="1" ht="14.45" customHeight="1">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+    </row>
+    <row r="5" spans="2:14" s="1" customFormat="1" ht="22.5">
+      <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="2:14" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B6" s="3" t="s">
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="2:14" s="1" customFormat="1" ht="22.5">
+      <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="9"/>
-    </row>
-    <row r="10" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E10" s="8" t="s">
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="2:14" s="1" customFormat="1">
+      <c r="F7" s="7"/>
+    </row>
+    <row r="10" spans="2:14" ht="27">
+      <c r="E10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="8" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E11" s="7" t="s">
+    <row r="11" spans="2:14" ht="27">
+      <c r="E11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="11">
-        <v>100</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="7" t="s">
+      <c r="F11" s="9">
+        <v>100</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E12" s="7" t="s">
+      <c r="J11" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="27">
+      <c r="E12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="11">
-        <v>100</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="7" t="s">
+      <c r="F12" s="9">
+        <v>100</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E13" s="7" t="s">
+      <c r="J12" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="27">
+      <c r="E13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="11">
-        <v>100</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="7" t="s">
+      <c r="F13" s="9">
+        <v>100</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E14" s="7" t="s">
+      <c r="J13" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="27">
+      <c r="E14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="11">
-        <v>100</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="7" t="s">
+      <c r="F14" s="9">
+        <v>100</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J14" s="11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E15" s="7" t="s">
+      <c r="J14" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="27">
+      <c r="E15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="11">
-        <v>100</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="7" t="s">
+      <c r="F15" s="9">
+        <v>100</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E16" s="6"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="5:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E17" s="14" t="s">
+      <c r="J15" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="27">
+      <c r="E16" s="4"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="5:10" ht="27">
+      <c r="E17" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="14" t="s">
+      <c r="F17" s="13">
+        <f>SUM(F11:F15)</f>
+        <v>500</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J17" s="15"/>
+      <c r="J17" s="13">
+        <f>SUBTOTAL(9,J11:J15)</f>
+        <v>500</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="E10:F15"/>
   <mergeCells count="3">
     <mergeCell ref="B2:N4"/>
     <mergeCell ref="B5:C5"/>

</xml_diff>